<commit_message>
Se realizan cambios para sanity semilla 8
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla8\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
-    <sheet name="Semilla 3" sheetId="2" r:id="rId2"/>
+    <sheet name="Semilla 9" sheetId="2" r:id="rId2"/>
+    <sheet name="Semilla 8" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="72">
   <si>
     <t>MSIDN</t>
   </si>
@@ -165,25 +166,82 @@
     <t>732111198172292</t>
   </si>
   <si>
-    <t>http://10.69.60.106:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
-    <t>http://10.69.60.107:8080/CRMPortal/auth/portal/default/Venta</t>
-  </si>
-  <si>
-    <t>http://10.69.60.106:8180/tigo-pos-web/index.jsp</t>
-  </si>
-  <si>
-    <t>10.69.60.103</t>
-  </si>
-  <si>
-    <t>10.69.60.102</t>
-  </si>
-  <si>
     <t>10.65.32.76</t>
   </si>
   <si>
-    <t>SIEBEL02</t>
+    <t>http://10.69.60.121:8180/tigo-pos-web/index.jsp</t>
+  </si>
+  <si>
+    <t>http://10.69.60.121:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.115</t>
+  </si>
+  <si>
+    <t>10.69.60.113</t>
+  </si>
+  <si>
+    <t>DESEPOS</t>
+  </si>
+  <si>
+    <t>DEV10G</t>
+  </si>
+  <si>
+    <t>212238780</t>
+  </si>
+  <si>
+    <t>250453824</t>
+  </si>
+  <si>
+    <t>664766732</t>
+  </si>
+  <si>
+    <t>220291650</t>
+  </si>
+  <si>
+    <t>125782671</t>
+  </si>
+  <si>
+    <t>http://10.69.60.123:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
+  </si>
+  <si>
+    <t>http://10.69.60.137:8180/tigo-pos-web/index.jsp</t>
+  </si>
+  <si>
+    <t>http://10.69.60.137:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.132</t>
+  </si>
+  <si>
+    <t>dev11g</t>
+  </si>
+  <si>
+    <t>10.69.60.130</t>
+  </si>
+  <si>
+    <t>SIEBEL05</t>
+  </si>
+  <si>
+    <t>SIEBEL</t>
+  </si>
+  <si>
+    <t>553312726</t>
+  </si>
+  <si>
+    <t>15377510</t>
+  </si>
+  <si>
+    <t>410614432</t>
+  </si>
+  <si>
+    <t>22368093</t>
+  </si>
+  <si>
+    <t>1050388676</t>
+  </si>
+  <si>
+    <t>http://10.69.60.140:8280/portal/login?initialURI=%2Fportal%2FCRMPortal%2FVenta</t>
   </si>
 </sst>
 </file>
@@ -820,7 +878,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -860,13 +918,13 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -900,6 +958,237 @@
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="21.36328125" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.08984375" customWidth="1"/>
+    <col min="4" max="4" width="28.08984375" customWidth="1"/>
+    <col min="5" max="5" width="42.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1">
+      <c r="A4" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -917,7 +1206,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>18</v>
@@ -931,7 +1220,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>20</v>
@@ -942,10 +1231,10 @@
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>23</v>
@@ -973,7 +1262,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -987,7 +1276,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>44</v>
@@ -1001,7 +1290,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1015,7 +1304,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1029,7 +1318,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Se implementa la clase ShhConnetions.java y la clase ReadFileCSV.java para la extraccion de la clave de asesor desde los logs del servidor. se adiciona los metodos de manejon en las clases CesionPortalCRMActions y CesionPortalPosCRMActions.java.
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla8\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8C0541-90C5-42C5-98F2-1E10137AAB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="77">
   <si>
     <t>MSIDN</t>
   </si>
@@ -242,12 +243,27 @@
   </si>
   <si>
     <t>http://10.69.60.140:8280/portal/login?initialURI=%2Fportal%2FCRMPortal%2FVenta</t>
+  </si>
+  <si>
+    <t>10.69.60.119</t>
+  </si>
+  <si>
+    <t>host ssh</t>
+  </si>
+  <si>
+    <t>usuario ssh</t>
+  </si>
+  <si>
+    <t>contraseña ssh</t>
+  </si>
+  <si>
+    <t>consulta_log</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -637,21 +653,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -862,11 +878,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -874,20 +890,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
-    <col min="3" max="3" width="24.6328125" customWidth="1"/>
-    <col min="4" max="4" width="31.1796875" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -1098,30 +1114,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
-    <col min="3" max="3" width="30.08984375" customWidth="1"/>
-    <col min="4" max="4" width="28.08984375" customWidth="1"/>
-    <col min="5" max="5" width="42.36328125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1137,17 +1153,26 @@
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1">
+      <c r="I1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
@@ -1172,8 +1197,17 @@
       <c r="H2" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1">
+      <c r="I2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1">
+    <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>49</v>
       </c>
@@ -1201,7 +1235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1">
+    <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>50</v>
       </c>
@@ -1215,7 +1249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1">
+    <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>50</v>
       </c>
@@ -1229,7 +1263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1">
+    <row r="7" spans="1:11" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
@@ -1243,7 +1277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1">
+    <row r="8" spans="1:11" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -1257,7 +1291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1">
+    <row r="9" spans="1:11" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1271,7 +1305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1">
+    <row r="10" spans="1:11" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1285,7 +1319,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1">
+    <row r="11" spans="1:11" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1299,7 +1333,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1">
+    <row r="12" spans="1:11" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1313,7 +1347,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1">
+    <row r="13" spans="1:11" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1329,11 +1363,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se realizan cambios para nuevos casos semilla 8
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla8\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8C0541-90C5-42C5-98F2-1E10137AAB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="102">
   <si>
     <t>MSIDN</t>
   </si>
@@ -188,21 +187,6 @@
     <t>DEV10G</t>
   </si>
   <si>
-    <t>212238780</t>
-  </si>
-  <si>
-    <t>250453824</t>
-  </si>
-  <si>
-    <t>664766732</t>
-  </si>
-  <si>
-    <t>220291650</t>
-  </si>
-  <si>
-    <t>125782671</t>
-  </si>
-  <si>
     <t>http://10.69.60.123:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
   </si>
   <si>
@@ -258,12 +242,102 @@
   </si>
   <si>
     <t>consulta_log</t>
+  </si>
+  <si>
+    <t>msisdn</t>
+  </si>
+  <si>
+    <t>msi</t>
+  </si>
+  <si>
+    <t>nip</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>portId</t>
+  </si>
+  <si>
+    <t>3043208091</t>
+  </si>
+  <si>
+    <t>732111324707274</t>
+  </si>
+  <si>
+    <t>3045981684</t>
+  </si>
+  <si>
+    <t>732111193278813</t>
+  </si>
+  <si>
+    <t>81684</t>
+  </si>
+  <si>
+    <t>1061520830</t>
+  </si>
+  <si>
+    <t>00002201108240181684</t>
+  </si>
+  <si>
+    <t>3043209773</t>
+  </si>
+  <si>
+    <t>732111324707275</t>
+  </si>
+  <si>
+    <t>3045984642</t>
+  </si>
+  <si>
+    <t>732111193278730</t>
+  </si>
+  <si>
+    <t>81670</t>
+  </si>
+  <si>
+    <t>111295346</t>
+  </si>
+  <si>
+    <t>00002201108240181670</t>
+  </si>
+  <si>
+    <t>3043209819</t>
+  </si>
+  <si>
+    <t>732111324707276</t>
+  </si>
+  <si>
+    <t>732111324707277</t>
+  </si>
+  <si>
+    <t>732111324707278</t>
+  </si>
+  <si>
+    <t>3043209863</t>
+  </si>
+  <si>
+    <t>139432597</t>
+  </si>
+  <si>
+    <t>309461124</t>
+  </si>
+  <si>
+    <t>160255294</t>
+  </si>
+  <si>
+    <t>705809003</t>
+  </si>
+  <si>
+    <t>268560134</t>
+  </si>
+  <si>
+    <t>3043209868</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -323,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -338,6 +412,12 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -653,21 +733,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -878,11 +958,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -890,20 +970,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -934,13 +1014,13 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -974,10 +1054,10 @@
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>15</v>
@@ -988,7 +1068,7 @@
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>51</v>
@@ -1002,7 +1082,7 @@
     </row>
     <row r="6" spans="1:8" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -1019,10 +1099,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -1047,7 +1127,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -1061,7 +1141,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>44</v>
@@ -1075,7 +1155,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1089,7 +1169,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>39</v>
@@ -1103,7 +1183,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>
@@ -1114,27 +1194,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
@@ -1162,22 +1242,16 @@
       <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>48</v>
@@ -1196,15 +1270,6 @@
       </c>
       <c r="H2" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1">
@@ -1234,6 +1299,15 @@
       <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
@@ -1248,6 +1322,15 @@
       <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
@@ -1284,11 +1367,26 @@
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1">
@@ -1296,13 +1394,28 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>78</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1">
@@ -1310,13 +1423,28 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>45</v>
+        <v>85</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1">
@@ -1324,13 +1452,13 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1">
@@ -1338,13 +1466,13 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1">
@@ -1352,22 +1480,36 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="7">
+        <v>709903476</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios para sanity semilla 8
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla8\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla8\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C53187E-1EE9-4970-B260-1E4292E4E74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="103">
   <si>
     <t>MSIDN</t>
   </si>
@@ -316,28 +317,31 @@
     <t>3043209863</t>
   </si>
   <si>
-    <t>139432597</t>
-  </si>
-  <si>
-    <t>309461124</t>
-  </si>
-  <si>
-    <t>160255294</t>
-  </si>
-  <si>
-    <t>705809003</t>
-  </si>
-  <si>
-    <t>268560134</t>
-  </si>
-  <si>
     <t>3043209868</t>
+  </si>
+  <si>
+    <t>3045981670</t>
+  </si>
+  <si>
+    <t>459399130</t>
+  </si>
+  <si>
+    <t>255188531</t>
+  </si>
+  <si>
+    <t>194936717</t>
+  </si>
+  <si>
+    <t>432694001</t>
+  </si>
+  <si>
+    <t>836898669</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -733,21 +737,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -958,11 +962,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -970,20 +974,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="31.1796875" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -1249,7 +1253,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>94</v>
@@ -1271,27 +1275,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" customWidth="1"/>
-    <col min="5" max="5" width="35.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
@@ -1471,7 +1475,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>77</v>
@@ -1500,7 +1504,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>84</v>
@@ -1529,7 +1533,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>77</v>
@@ -1543,10 +1547,10 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>92</v>
@@ -1557,10 +1561,10 @@
         <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>94</v>
@@ -1571,7 +1575,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="7">
-        <v>709903476</v>
+        <v>920626579</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>95</v>
@@ -1582,11 +1586,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>